<commit_message>
Update with program to extract csvs from excel files with line breaks.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/MEADS/2011_SAR DataDraw_MEADS.xlsx
+++ b/FOIA SAR data/MEADS/2011_SAR DataDraw_MEADS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2015-09 Joint Development\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg Sanders\Documents\Development\R-scripts-and-data\FOIA SAR data\MEADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CostSummary" sheetId="1" r:id="rId1"/>
@@ -1135,7 +1135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1368,6 +1368,58 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="13"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="9"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="14"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1386,12 +1438,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1402,6 +1448,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1443,46 +1495,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="13"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="9"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="14"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1797,11 +1815,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1826,76 +1842,76 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="88" t="s">
+      <c r="A3" s="104"/>
+      <c r="B3" s="106" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="89"/>
+      <c r="C3" s="107"/>
       <c r="D3" s="30"/>
       <c r="E3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="92"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="108"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="87"/>
-      <c r="B4" s="90"/>
-      <c r="C4" s="91"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="113"/>
       <c r="D4" s="31"/>
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="93"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="95"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="111"/>
     </row>
     <row r="5" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="92"/>
-      <c r="E5" s="84" t="s">
+      <c r="D5" s="108"/>
+      <c r="E5" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="96"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="114"/>
     </row>
     <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="84" t="s">
+      <c r="A6" s="115"/>
+      <c r="B6" s="117"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="84" t="s">
+      <c r="G6" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="102" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
+      <c r="A7" s="116"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="114"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -2199,76 +2215,76 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="86"/>
-      <c r="B21" s="88" t="s">
+      <c r="A21" s="104"/>
+      <c r="B21" s="106" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="89"/>
-      <c r="D21" s="92"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="108"/>
       <c r="E21" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="F21" s="88" t="s">
+      <c r="F21" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="89"/>
-      <c r="H21" s="92"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="108"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="87"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="96"/>
+      <c r="A22" s="105"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="114"/>
       <c r="E22" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="93"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="95"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="111"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="84" t="s">
+      <c r="A23" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="92"/>
-      <c r="E23" s="84" t="s">
+      <c r="D23" s="108"/>
+      <c r="E23" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="90"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="96"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="114"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="97"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="84" t="s">
+      <c r="A24" s="115"/>
+      <c r="B24" s="117"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="115"/>
+      <c r="F24" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="84" t="s">
+      <c r="G24" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="H24" s="84" t="s">
+      <c r="H24" s="102" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="98"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="116"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
@@ -2571,10 +2587,10 @@
       <c r="B38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="84" t="s">
+      <c r="C38" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="84" t="s">
+      <c r="D38" s="102" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2585,8 +2601,8 @@
       <c r="B39" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
+      <c r="C39" s="103"/>
+      <c r="D39" s="103"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -2630,432 +2646,424 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="86"/>
-      <c r="B45" s="88" t="s">
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="104"/>
+      <c r="B46" s="106" t="s">
         <v>161</v>
       </c>
-      <c r="C45" s="89"/>
-      <c r="D45" s="92"/>
-      <c r="E45" s="80" t="s">
+      <c r="C46" s="107"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="F45" s="88" t="s">
+      <c r="F46" s="106" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="89"/>
-      <c r="H45" s="92"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="87"/>
-      <c r="B46" s="90"/>
-      <c r="C46" s="91"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="81" t="s">
+      <c r="G46" s="107"/>
+      <c r="H46" s="108"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="105"/>
+      <c r="B47" s="112"/>
+      <c r="C47" s="113"/>
+      <c r="D47" s="114"/>
+      <c r="E47" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="F46" s="93"/>
-      <c r="G46" s="94"/>
-      <c r="H46" s="95"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="84" t="s">
+      <c r="F47" s="109"/>
+      <c r="G47" s="110"/>
+      <c r="H47" s="111"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="84" t="s">
+      <c r="B48" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="88" t="s">
+      <c r="C48" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="D47" s="92"/>
-      <c r="E47" s="84" t="s">
+      <c r="D48" s="108"/>
+      <c r="E48" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="F47" s="90"/>
-      <c r="G47" s="91"/>
-      <c r="H47" s="96"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="97"/>
-      <c r="B48" s="99"/>
-      <c r="C48" s="93"/>
-      <c r="D48" s="95"/>
-      <c r="E48" s="97"/>
-      <c r="F48" s="84" t="s">
+      <c r="F48" s="112"/>
+      <c r="G48" s="113"/>
+      <c r="H48" s="114"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="115"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="111"/>
+      <c r="E49" s="115"/>
+      <c r="F49" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="84" t="s">
+      <c r="G49" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="H48" s="84" t="s">
+      <c r="H49" s="102" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="98"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="96"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="98"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="5">
-        <v>460.9</v>
-      </c>
-      <c r="C50" s="5">
-        <v>460.9</v>
-      </c>
-      <c r="D50" s="5">
-        <v>530</v>
-      </c>
-      <c r="E50" s="5">
-        <v>703.9</v>
-      </c>
-      <c r="F50" s="5">
-        <v>482</v>
-      </c>
-      <c r="G50" s="5">
-        <v>482</v>
-      </c>
-      <c r="H50" s="5">
-        <v>788.2</v>
-      </c>
+    <row r="50" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="116"/>
+      <c r="B50" s="103"/>
+      <c r="C50" s="112"/>
+      <c r="D50" s="114"/>
+      <c r="E50" s="116"/>
+      <c r="F50" s="116"/>
+      <c r="G50" s="116"/>
+      <c r="H50" s="116"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="5">
+        <v>460.9</v>
+      </c>
+      <c r="C51" s="5">
+        <v>460.9</v>
+      </c>
+      <c r="D51" s="5">
+        <v>530</v>
+      </c>
+      <c r="E51" s="5">
+        <v>703.9</v>
+      </c>
+      <c r="F51" s="5">
+        <v>482</v>
+      </c>
+      <c r="G51" s="5">
+        <v>482</v>
+      </c>
+      <c r="H51" s="5">
+        <v>788.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B52" s="5">
         <v>5760</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C52" s="5">
         <v>5760</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D52" s="5">
         <v>6336</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E52" s="5">
         <v>6165.7</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F52" s="5">
         <v>7574</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G52" s="5">
         <v>7574</v>
       </c>
-      <c r="H51" s="5">
+      <c r="H52" s="5">
         <v>8986.9</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B52" s="110">
+      <c r="B53" s="87">
         <v>5252.9</v>
       </c>
-      <c r="C52" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="110">
+      <c r="C53" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="87">
         <v>5662.5</v>
       </c>
-      <c r="F52" s="110">
+      <c r="F53" s="87">
         <v>6914.8</v>
       </c>
-      <c r="G52" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="H52" s="110">
+      <c r="G53" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="87">
         <v>8257.9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" s="110">
-        <v>5252.9</v>
-      </c>
-      <c r="C53" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="110">
-        <v>5590.5</v>
-      </c>
-      <c r="F53" s="110">
-        <v>6914.8</v>
-      </c>
-      <c r="G53" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="H53" s="110">
-        <v>8170</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="87">
+        <v>5252.9</v>
+      </c>
+      <c r="C54" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="87">
+        <v>5590.5</v>
+      </c>
+      <c r="F54" s="87">
+        <v>6914.8</v>
+      </c>
+      <c r="G54" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="87">
+        <v>8170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="110">
-        <v>0</v>
-      </c>
-      <c r="C54" s="110" t="s">
+      <c r="B55" s="87">
+        <v>0</v>
+      </c>
+      <c r="C55" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="D54" s="110" t="s">
+      <c r="D55" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="E54" s="110">
+      <c r="E55" s="87">
         <v>72</v>
       </c>
-      <c r="F54" s="110">
-        <v>0</v>
-      </c>
-      <c r="G54" s="110" t="s">
+      <c r="F55" s="87">
+        <v>0</v>
+      </c>
+      <c r="G55" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="H54" s="110">
+      <c r="H55" s="87">
         <v>87.9</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="110">
+      <c r="B56" s="87">
         <v>507.1</v>
       </c>
-      <c r="C55" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" s="110">
+      <c r="C56" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="87">
         <v>503.2</v>
       </c>
-      <c r="F55" s="110">
+      <c r="F56" s="87">
         <v>659.2</v>
       </c>
-      <c r="G55" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" s="110">
+      <c r="G56" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="87">
         <v>729</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="110">
+      <c r="B57" s="87">
         <v>507.1</v>
       </c>
-      <c r="C56" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" s="110">
+      <c r="C57" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="87">
         <v>503.2</v>
       </c>
-      <c r="F56" s="110">
+      <c r="F57" s="87">
         <v>659.2</v>
       </c>
-      <c r="G56" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" s="110">
+      <c r="G57" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="87">
         <v>729</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="110">
-        <v>0</v>
-      </c>
-      <c r="C57" s="110" t="s">
+      <c r="B58" s="87">
+        <v>0</v>
+      </c>
+      <c r="C58" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="D57" s="110" t="s">
+      <c r="D58" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="E57" s="110">
-        <v>0</v>
-      </c>
-      <c r="F57" s="110">
-        <v>0</v>
-      </c>
-      <c r="G57" s="110" t="s">
+      <c r="E58" s="87">
+        <v>0</v>
+      </c>
+      <c r="F58" s="87">
+        <v>0</v>
+      </c>
+      <c r="G58" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="H57" s="110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+      <c r="H58" s="87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="5">
-        <v>0</v>
-      </c>
-      <c r="C58" s="5">
-        <v>0</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="5">
-        <v>0</v>
-      </c>
-      <c r="F58" s="5">
-        <v>0</v>
-      </c>
-      <c r="G58" s="5">
-        <v>0</v>
-      </c>
-      <c r="H58" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+      <c r="B59" s="5">
+        <v>0</v>
+      </c>
+      <c r="C59" s="5">
+        <v>0</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="5">
+        <v>0</v>
+      </c>
+      <c r="F59" s="5">
+        <v>0</v>
+      </c>
+      <c r="G59" s="5">
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="5">
-        <v>0</v>
-      </c>
-      <c r="C59" s="5">
-        <v>0</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" s="5">
-        <v>0</v>
-      </c>
-      <c r="F59" s="5">
-        <v>0</v>
-      </c>
-      <c r="G59" s="5">
-        <v>0</v>
-      </c>
-      <c r="H59" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="B60" s="5">
+        <v>0</v>
+      </c>
+      <c r="C60" s="5">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0</v>
+      </c>
+      <c r="F60" s="5">
+        <v>0</v>
+      </c>
+      <c r="G60" s="5">
+        <v>0</v>
+      </c>
+      <c r="H60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="110">
+      <c r="B61" s="87">
         <v>6220.9</v>
       </c>
-      <c r="C60" s="110">
+      <c r="C61" s="87">
         <v>6220.9</v>
       </c>
-      <c r="D60" s="110" t="s">
+      <c r="D61" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="110">
+      <c r="E61" s="87">
         <v>6869.6</v>
       </c>
-      <c r="F60" s="110">
+      <c r="F61" s="87">
         <v>8056</v>
       </c>
-      <c r="G60" s="110">
+      <c r="G61" s="87">
         <v>8056</v>
       </c>
-      <c r="H60" s="110">
+      <c r="H61" s="87">
         <v>9775.1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="5"/>
-    </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24"/>
-      <c r="B62" s="80" t="s">
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="16"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="24"/>
+      <c r="B63" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="84" t="s">
+      <c r="C63" s="102" t="s">
         <v>154</v>
       </c>
-      <c r="D62" s="84" t="s">
+      <c r="D63" s="102" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="79" t="s">
+    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="B63" s="81" t="s">
+      <c r="B64" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="85"/>
-      <c r="D63" s="85"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="C64" s="103"/>
+      <c r="D64" s="103"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="23">
-        <v>0</v>
-      </c>
-      <c r="C64" s="23">
-        <v>0</v>
-      </c>
-      <c r="D64" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+      <c r="B65" s="23">
+        <v>0</v>
+      </c>
+      <c r="C65" s="23">
+        <v>0</v>
+      </c>
+      <c r="D65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B65" s="23">
-        <v>1528</v>
-      </c>
-      <c r="C65" s="23">
-        <v>1528</v>
-      </c>
-      <c r="D65" s="5">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="B66" s="23">
         <v>1528</v>
@@ -3064,6 +3072,20 @@
         <v>1528</v>
       </c>
       <c r="D66" s="5">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" s="23">
+        <v>1528</v>
+      </c>
+      <c r="C67" s="23">
+        <v>1528</v>
+      </c>
+      <c r="D67" s="5">
         <v>1528</v>
       </c>
     </row>
@@ -3091,18 +3113,18 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="F45:H47"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="B45:D46"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="F46:H48"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:D50"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="B46:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3113,8 +3135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K944"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N146" sqref="N146"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3130,46 +3152,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="127" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="96"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="128" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="101"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="128" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
@@ -3180,7 +3202,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="100" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="21"/>
@@ -3210,7 +3232,7 @@
       <c r="H5" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="101" t="s">
         <v>34</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -3242,7 +3264,7 @@
       <c r="H6" s="10">
         <v>0</v>
       </c>
-      <c r="I6" s="109">
+      <c r="I6" s="86">
         <v>0</v>
       </c>
       <c r="J6" s="11">
@@ -3253,7 +3275,7 @@
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="109">
+      <c r="B7" s="86">
         <v>0</v>
       </c>
       <c r="C7" s="8">
@@ -3285,7 +3307,7 @@
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="109">
+      <c r="B8" s="86">
         <v>0</v>
       </c>
       <c r="C8" s="10">
@@ -3306,7 +3328,7 @@
       <c r="H8" s="10">
         <v>0</v>
       </c>
-      <c r="I8" s="109">
+      <c r="I8" s="86">
         <v>0</v>
       </c>
       <c r="J8" s="10">
@@ -3454,32 +3476,32 @@
       <c r="J13" s="63"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="118" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="100"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="100"/>
-      <c r="J14" s="101"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
+      <c r="F14" s="118"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="119"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="B15" s="100"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="100"/>
-      <c r="I15" s="100"/>
-      <c r="J15" s="101"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="119"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
@@ -3563,7 +3585,7 @@
       <c r="A19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="109">
+      <c r="B19" s="86">
         <v>0</v>
       </c>
       <c r="C19" s="10">
@@ -3595,7 +3617,7 @@
       <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="109">
+      <c r="B20" s="86">
         <v>0</v>
       </c>
       <c r="C20" s="10">
@@ -3990,33 +4012,33 @@
       <c r="K32" s="12"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="100" t="s">
+      <c r="A33" s="118" t="s">
         <v>174</v>
       </c>
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="100"/>
-      <c r="I33" s="100"/>
-      <c r="J33" s="101"/>
+      <c r="B33" s="118"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="119"/>
       <c r="K33" s="12"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="100" t="s">
+      <c r="A34" s="118" t="s">
         <v>169</v>
       </c>
-      <c r="B34" s="100"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="100"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="100"/>
-      <c r="J34" s="101"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="118"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="118"/>
+      <c r="I34" s="118"/>
+      <c r="J34" s="119"/>
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -4092,7 +4114,7 @@
       <c r="H37" s="10">
         <v>0</v>
       </c>
-      <c r="I37" s="109">
+      <c r="I37" s="86">
         <v>0</v>
       </c>
       <c r="J37" s="11">
@@ -4104,7 +4126,7 @@
       <c r="A38" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="109">
+      <c r="B38" s="86">
         <v>0</v>
       </c>
       <c r="C38" s="8">
@@ -4535,17 +4557,17 @@
       <c r="K51" s="12"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="100" t="s">
+      <c r="A52" s="118" t="s">
         <v>176</v>
       </c>
-      <c r="B52" s="100"/>
-      <c r="C52" s="100"/>
-      <c r="D52" s="100"/>
-      <c r="E52" s="100"/>
-      <c r="F52" s="100"/>
-      <c r="G52" s="100"/>
-      <c r="H52" s="100"/>
-      <c r="I52" s="101"/>
+      <c r="B52" s="118"/>
+      <c r="C52" s="118"/>
+      <c r="D52" s="118"/>
+      <c r="E52" s="118"/>
+      <c r="F52" s="118"/>
+      <c r="G52" s="118"/>
+      <c r="H52" s="118"/>
+      <c r="I52" s="119"/>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
     </row>
@@ -4873,17 +4895,17 @@
       <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="100" t="s">
+      <c r="A66" s="118" t="s">
         <v>177</v>
       </c>
-      <c r="B66" s="100"/>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="100"/>
-      <c r="H66" s="100"/>
-      <c r="I66" s="101"/>
+      <c r="B66" s="118"/>
+      <c r="C66" s="118"/>
+      <c r="D66" s="118"/>
+      <c r="E66" s="118"/>
+      <c r="F66" s="118"/>
+      <c r="G66" s="118"/>
+      <c r="H66" s="118"/>
+      <c r="I66" s="119"/>
     </row>
     <row r="67" spans="1:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="27" t="s">
@@ -5209,72 +5231,72 @@
       <c r="H79" s="12"/>
     </row>
     <row r="80" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="100" t="s">
+      <c r="A80" s="118" t="s">
         <v>178</v>
       </c>
-      <c r="B80" s="100"/>
-      <c r="C80" s="100"/>
-      <c r="D80" s="100"/>
-      <c r="E80" s="100"/>
-      <c r="F80" s="100"/>
-      <c r="G80" s="100"/>
-      <c r="H80" s="100"/>
+      <c r="B80" s="118"/>
+      <c r="C80" s="118"/>
+      <c r="D80" s="118"/>
+      <c r="E80" s="118"/>
+      <c r="F80" s="118"/>
+      <c r="G80" s="118"/>
+      <c r="H80" s="118"/>
     </row>
     <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="84" t="s">
+      <c r="A81" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="84" t="s">
+      <c r="B81" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="84" t="s">
+      <c r="C81" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="D81" s="84" t="s">
+      <c r="D81" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="E81" s="84" t="s">
+      <c r="E81" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="F81" s="84" t="s">
+      <c r="F81" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="G81" s="84" t="s">
+      <c r="G81" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="H81" s="84" t="s">
+      <c r="H81" s="102" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="99"/>
-      <c r="B82" s="99"/>
-      <c r="C82" s="99"/>
-      <c r="D82" s="99"/>
-      <c r="E82" s="99"/>
-      <c r="F82" s="99"/>
-      <c r="G82" s="99"/>
-      <c r="H82" s="99"/>
+      <c r="A82" s="117"/>
+      <c r="B82" s="117"/>
+      <c r="C82" s="117"/>
+      <c r="D82" s="117"/>
+      <c r="E82" s="117"/>
+      <c r="F82" s="117"/>
+      <c r="G82" s="117"/>
+      <c r="H82" s="117"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="99"/>
-      <c r="B83" s="99"/>
-      <c r="C83" s="99"/>
-      <c r="D83" s="99"/>
-      <c r="E83" s="99"/>
-      <c r="F83" s="99"/>
-      <c r="G83" s="99"/>
-      <c r="H83" s="99"/>
+      <c r="A83" s="117"/>
+      <c r="B83" s="117"/>
+      <c r="C83" s="117"/>
+      <c r="D83" s="117"/>
+      <c r="E83" s="117"/>
+      <c r="F83" s="117"/>
+      <c r="G83" s="117"/>
+      <c r="H83" s="117"/>
     </row>
     <row r="84" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="85"/>
-      <c r="B84" s="85"/>
-      <c r="C84" s="85"/>
-      <c r="D84" s="85"/>
-      <c r="E84" s="85"/>
-      <c r="F84" s="85"/>
-      <c r="G84" s="85"/>
-      <c r="H84" s="85"/>
+      <c r="A84" s="103"/>
+      <c r="B84" s="103"/>
+      <c r="C84" s="103"/>
+      <c r="D84" s="103"/>
+      <c r="E84" s="103"/>
+      <c r="F84" s="103"/>
+      <c r="G84" s="103"/>
+      <c r="H84" s="103"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
@@ -5564,16 +5586,16 @@
     </row>
     <row r="96" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="97" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="100" t="s">
+      <c r="A97" s="118" t="s">
         <v>179</v>
       </c>
-      <c r="B97" s="100"/>
-      <c r="C97" s="100"/>
-      <c r="D97" s="100"/>
-      <c r="E97" s="100"/>
-      <c r="F97" s="100"/>
-      <c r="G97" s="100"/>
-      <c r="H97" s="100"/>
+      <c r="B97" s="118"/>
+      <c r="C97" s="118"/>
+      <c r="D97" s="118"/>
+      <c r="E97" s="118"/>
+      <c r="F97" s="118"/>
+      <c r="G97" s="118"/>
+      <c r="H97" s="118"/>
     </row>
     <row r="98" spans="1:8" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="27" t="s">
@@ -5889,16 +5911,16 @@
     </row>
     <row r="110" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="100" t="s">
+      <c r="A111" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="B111" s="100"/>
-      <c r="C111" s="100"/>
-      <c r="D111" s="100"/>
-      <c r="E111" s="100"/>
-      <c r="F111" s="100"/>
-      <c r="G111" s="100"/>
-      <c r="H111" s="100"/>
+      <c r="B111" s="118"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="118"/>
+      <c r="E111" s="118"/>
+      <c r="F111" s="118"/>
+      <c r="G111" s="118"/>
+      <c r="H111" s="118"/>
     </row>
     <row r="112" spans="1:8" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="27" t="s">
@@ -5945,7 +5967,7 @@
       <c r="F113" s="10">
         <v>75</v>
       </c>
-      <c r="G113" s="109" t="s">
+      <c r="G113" s="86" t="s">
         <v>6</v>
       </c>
       <c r="H113" s="10">
@@ -5971,7 +5993,7 @@
       <c r="F114" s="10">
         <v>12.9</v>
       </c>
-      <c r="G114" s="109" t="s">
+      <c r="G114" s="86" t="s">
         <v>6</v>
       </c>
       <c r="H114" s="10">
@@ -6529,16 +6551,16 @@
       <c r="I136" s="69"/>
     </row>
     <row r="137" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="100" t="s">
+      <c r="A137" s="118" t="s">
         <v>187</v>
       </c>
-      <c r="B137" s="100"/>
-      <c r="C137" s="100"/>
-      <c r="D137" s="100"/>
-      <c r="E137" s="100"/>
-      <c r="F137" s="100"/>
-      <c r="G137" s="100"/>
-      <c r="H137" s="100"/>
+      <c r="B137" s="118"/>
+      <c r="C137" s="118"/>
+      <c r="D137" s="118"/>
+      <c r="E137" s="118"/>
+      <c r="F137" s="118"/>
+      <c r="G137" s="118"/>
+      <c r="H137" s="118"/>
       <c r="I137" s="69"/>
     </row>
     <row r="138" spans="1:9" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -7108,10 +7130,10 @@
       <c r="F159" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G159" s="109">
+      <c r="G159" s="86">
         <v>6.6</v>
       </c>
-      <c r="H159" s="109">
+      <c r="H159" s="86">
         <v>6.6</v>
       </c>
     </row>
@@ -7134,10 +7156,10 @@
       <c r="F160" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G160" s="109">
+      <c r="G160" s="86">
         <v>6.5</v>
       </c>
-      <c r="H160" s="109">
+      <c r="H160" s="86">
         <v>6.5</v>
       </c>
     </row>
@@ -7235,12 +7257,9 @@
     <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="944" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A1:J1"/>
+  <mergeCells count="18">
     <mergeCell ref="A52:I52"/>
     <mergeCell ref="A80:H80"/>
-    <mergeCell ref="A2:J2"/>
     <mergeCell ref="A14:J14"/>
     <mergeCell ref="A15:J15"/>
     <mergeCell ref="A33:J33"/>
@@ -7268,7 +7287,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7279,11 +7298,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="118" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="119"/>
     </row>
     <row r="2" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
@@ -7345,11 +7364,11 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="118" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="100"/>
-      <c r="C9" s="101"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="119"/>
     </row>
     <row r="10" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
@@ -7430,7 +7449,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7452,8 +7471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95:I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7515,7 +7534,7 @@
       <c r="C5" s="9">
         <v>2758.8</v>
       </c>
-      <c r="D5" s="114"/>
+      <c r="D5" s="91"/>
     </row>
     <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
@@ -7527,7 +7546,7 @@
       <c r="C6" s="9">
         <v>0</v>
       </c>
-      <c r="D6" s="114"/>
+      <c r="D6" s="91"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
@@ -7561,7 +7580,7 @@
       <c r="C9" s="9">
         <v>0</v>
       </c>
-      <c r="D9" s="114"/>
+      <c r="D9" s="91"/>
     </row>
     <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
@@ -7573,7 +7592,7 @@
       <c r="C10" s="9">
         <v>0</v>
       </c>
-      <c r="D10" s="114"/>
+      <c r="D10" s="91"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
@@ -7623,13 +7642,13 @@
       <c r="A16" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="111">
+      <c r="B16" s="88">
         <v>16530.5</v>
       </c>
       <c r="C16" s="37">
         <v>2758.8</v>
       </c>
-      <c r="D16" s="112"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
@@ -7638,19 +7657,19 @@
       <c r="B17" s="19">
         <v>48</v>
       </c>
-      <c r="C17" s="113">
-        <v>0</v>
-      </c>
-      <c r="D17" s="112"/>
+      <c r="C17" s="90">
+        <v>0</v>
+      </c>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="111">
+      <c r="B18" s="88">
         <v>344.38499999999999</v>
       </c>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="90" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="19" t="s">
@@ -7667,13 +7686,13 @@
       <c r="A20" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="111">
+      <c r="B20" s="88">
         <v>11999.1</v>
       </c>
       <c r="C20" s="9">
         <v>0</v>
       </c>
-      <c r="D20" s="112"/>
+      <c r="D20" s="89"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
@@ -7685,13 +7704,13 @@
       <c r="C21" s="9">
         <v>0</v>
       </c>
-      <c r="D21" s="112"/>
+      <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="111">
+      <c r="B22" s="88">
         <v>249.98099999999999</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -7707,14 +7726,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="102" t="s">
+      <c r="C25" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="D25" s="101"/>
-      <c r="E25" s="102" t="s">
+      <c r="D25" s="119"/>
+      <c r="E25" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="101"/>
+      <c r="F25" s="119"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="27" t="s">
@@ -7737,7 +7756,7 @@
       <c r="A27" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="115">
+      <c r="B27" s="92">
         <v>38200</v>
       </c>
       <c r="C27" s="9">
@@ -7757,7 +7776,7 @@
       <c r="A28" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="115">
+      <c r="B28" s="92">
         <v>38200</v>
       </c>
       <c r="C28" s="9">
@@ -7817,7 +7836,7 @@
       <c r="A31" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="115">
+      <c r="B31" s="92">
         <v>38200</v>
       </c>
       <c r="C31" s="9">
@@ -7837,7 +7856,7 @@
       <c r="A32" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="115">
+      <c r="B32" s="92">
         <v>40513</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -7857,7 +7876,7 @@
       <c r="A33" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="115">
+      <c r="B33" s="92">
         <v>40878</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -7878,17 +7897,17 @@
       <c r="A35" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="102" t="s">
+      <c r="B35" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="101"/>
-      <c r="J35" s="84" t="s">
+      <c r="C35" s="118"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="119"/>
+      <c r="J35" s="102" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7920,7 +7939,7 @@
       <c r="I36" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J36" s="85"/>
+      <c r="J36" s="103"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
@@ -7962,17 +7981,17 @@
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41"/>
-      <c r="B40" s="102" t="s">
+      <c r="B40" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="100"/>
-      <c r="D40" s="100"/>
-      <c r="E40" s="100"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="100"/>
-      <c r="H40" s="100"/>
-      <c r="I40" s="101"/>
-      <c r="J40" s="84" t="s">
+      <c r="C40" s="118"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+      <c r="I40" s="119"/>
+      <c r="J40" s="102" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8004,7 +8023,7 @@
       <c r="I41" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J41" s="85"/>
+      <c r="J41" s="103"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
@@ -8045,13 +8064,13 @@
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="102" t="s">
+      <c r="A45" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="100"/>
-      <c r="C45" s="100"/>
-      <c r="D45" s="100"/>
-      <c r="E45" s="101"/>
+      <c r="B45" s="118"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="119"/>
     </row>
     <row r="46" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
@@ -8094,13 +8113,13 @@
       <c r="B48" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="115">
+      <c r="C48" s="92">
         <v>38200</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="115">
+      <c r="E48" s="92">
         <v>38200</v>
       </c>
     </row>
@@ -8111,13 +8130,13 @@
       <c r="B49" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="115">
+      <c r="C49" s="92">
         <v>41214</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="115">
+      <c r="E49" s="92">
         <v>41214</v>
       </c>
     </row>
@@ -8128,13 +8147,13 @@
       <c r="B50" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="115">
+      <c r="C50" s="92">
         <v>42979</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="115">
+      <c r="E50" s="92">
         <v>42979</v>
       </c>
     </row>
@@ -8229,31 +8248,31 @@
       <c r="A60" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="116">
+      <c r="B60" s="93">
         <v>6220.9</v>
       </c>
       <c r="C60" s="37">
         <v>6869.6</v>
       </c>
-      <c r="D60" s="112"/>
+      <c r="D60" s="89"/>
     </row>
     <row r="61" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B61" s="117">
+      <c r="B61" s="94">
         <v>1528</v>
       </c>
       <c r="C61" s="38">
         <v>1528</v>
       </c>
-      <c r="D61" s="112"/>
+      <c r="D61" s="89"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="117">
+      <c r="B62" s="94">
         <v>4.0709999999999997</v>
       </c>
       <c r="C62" s="38">
@@ -8273,31 +8292,31 @@
       <c r="A64" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="116">
+      <c r="B64" s="93">
         <v>5760</v>
       </c>
       <c r="C64" s="37">
         <v>6165.7</v>
       </c>
-      <c r="D64" s="112"/>
+      <c r="D64" s="89"/>
     </row>
     <row r="65" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="117">
+      <c r="B65" s="94">
         <v>1528</v>
       </c>
       <c r="C65" s="38">
         <v>1528</v>
       </c>
-      <c r="D65" s="112"/>
+      <c r="D65" s="89"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="117">
+      <c r="B66" s="94">
         <v>3.77</v>
       </c>
       <c r="C66" s="38">
@@ -8341,31 +8360,31 @@
       <c r="A71" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B71" s="116">
+      <c r="B71" s="93">
         <v>6220.9</v>
       </c>
       <c r="C71" s="37">
         <v>6869.6</v>
       </c>
-      <c r="D71" s="112"/>
+      <c r="D71" s="89"/>
     </row>
     <row r="72" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B72" s="117">
+      <c r="B72" s="94">
         <v>1528</v>
       </c>
       <c r="C72" s="38">
         <v>1528</v>
       </c>
-      <c r="D72" s="112"/>
+      <c r="D72" s="89"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="117">
+      <c r="B73" s="94">
         <v>4.0709999999999997</v>
       </c>
       <c r="C73" s="38">
@@ -8385,31 +8404,31 @@
       <c r="A75" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B75" s="116">
+      <c r="B75" s="93">
         <v>5760</v>
       </c>
       <c r="C75" s="37">
         <v>6165.7</v>
       </c>
-      <c r="D75" s="112"/>
+      <c r="D75" s="89"/>
     </row>
     <row r="76" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B76" s="117">
+      <c r="B76" s="94">
         <v>1528</v>
       </c>
       <c r="C76" s="38">
         <v>1528</v>
       </c>
-      <c r="D76" s="112"/>
+      <c r="D76" s="89"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B77" s="117">
+      <c r="B77" s="94">
         <v>3.77</v>
       </c>
       <c r="C77" s="38">
@@ -8425,14 +8444,14 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C80" s="102" t="s">
+      <c r="C80" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="D80" s="101"/>
-      <c r="E80" s="102" t="s">
+      <c r="D80" s="119"/>
+      <c r="E80" s="120" t="s">
         <v>16</v>
       </c>
-      <c r="F80" s="101"/>
+      <c r="F80" s="119"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="27" t="s">
@@ -8455,7 +8474,7 @@
       <c r="A82" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B82" s="115">
+      <c r="B82" s="92">
         <v>38200</v>
       </c>
       <c r="C82" s="9">
@@ -8475,7 +8494,7 @@
       <c r="A83" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B83" s="115">
+      <c r="B83" s="92">
         <v>38200</v>
       </c>
       <c r="C83" s="9">
@@ -8535,7 +8554,7 @@
       <c r="A86" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B86" s="115">
+      <c r="B86" s="92">
         <v>38200</v>
       </c>
       <c r="C86" s="9">
@@ -8555,7 +8574,7 @@
       <c r="A87" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B87" s="115">
+      <c r="B87" s="92">
         <v>40513</v>
       </c>
       <c r="C87" s="9">
@@ -8575,7 +8594,7 @@
       <c r="A88" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B88" s="115">
+      <c r="B88" s="92">
         <v>40878</v>
       </c>
       <c r="C88" s="9">
@@ -8596,17 +8615,17 @@
       <c r="A90" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B90" s="102" t="s">
+      <c r="B90" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="C90" s="100"/>
-      <c r="D90" s="100"/>
-      <c r="E90" s="100"/>
-      <c r="F90" s="100"/>
-      <c r="G90" s="100"/>
-      <c r="H90" s="100"/>
-      <c r="I90" s="101"/>
-      <c r="J90" s="84" t="s">
+      <c r="C90" s="118"/>
+      <c r="D90" s="118"/>
+      <c r="E90" s="118"/>
+      <c r="F90" s="118"/>
+      <c r="G90" s="118"/>
+      <c r="H90" s="118"/>
+      <c r="I90" s="119"/>
+      <c r="J90" s="102" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8638,7 +8657,7 @@
       <c r="I91" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J91" s="85"/>
+      <c r="J91" s="103"/>
     </row>
     <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="27" t="s">
@@ -8680,17 +8699,17 @@
     <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="41"/>
-      <c r="B95" s="102" t="s">
+      <c r="B95" s="120" t="s">
         <v>77</v>
       </c>
-      <c r="C95" s="100"/>
-      <c r="D95" s="100"/>
-      <c r="E95" s="100"/>
-      <c r="F95" s="100"/>
-      <c r="G95" s="100"/>
-      <c r="H95" s="100"/>
-      <c r="I95" s="101"/>
-      <c r="J95" s="84" t="s">
+      <c r="C95" s="118"/>
+      <c r="D95" s="118"/>
+      <c r="E95" s="118"/>
+      <c r="F95" s="118"/>
+      <c r="G95" s="118"/>
+      <c r="H95" s="118"/>
+      <c r="I95" s="119"/>
+      <c r="J95" s="102" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8722,7 +8741,7 @@
       <c r="I96" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J96" s="85"/>
+      <c r="J96" s="103"/>
     </row>
     <row r="97" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="27" t="s">
@@ -8763,13 +8782,13 @@
     </row>
     <row r="99" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="102" t="s">
+      <c r="A100" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="B100" s="100"/>
-      <c r="C100" s="100"/>
-      <c r="D100" s="100"/>
-      <c r="E100" s="101"/>
+      <c r="B100" s="118"/>
+      <c r="C100" s="118"/>
+      <c r="D100" s="118"/>
+      <c r="E100" s="119"/>
     </row>
     <row r="101" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="27" t="s">
@@ -8846,13 +8865,13 @@
       <c r="B105" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C105" s="115">
+      <c r="C105" s="92">
         <v>40603</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E105" s="115">
+      <c r="E105" s="92">
         <v>42248</v>
       </c>
     </row>
@@ -8933,8 +8952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:E78"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8952,22 +8971,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="120" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="120" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="101"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="119"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
@@ -9336,13 +9355,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="102" t="s">
+      <c r="A28" s="120" t="s">
         <v>204</v>
       </c>
-      <c r="B28" s="100"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="101"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="119"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
@@ -9508,16 +9527,16 @@
       <c r="A39" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="118">
+      <c r="B39" s="95">
         <v>-1730.9</v>
       </c>
-      <c r="C39" s="118">
+      <c r="C39" s="95">
         <v>-11920.1</v>
       </c>
-      <c r="D39" s="118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="118">
+      <c r="D39" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="95">
         <v>-13651</v>
       </c>
     </row>
@@ -9525,10 +9544,10 @@
       <c r="A40" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="119"/>
-      <c r="C40" s="119"/>
-      <c r="D40" s="119"/>
-      <c r="E40" s="119"/>
+      <c r="B40" s="96"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
@@ -9653,16 +9672,16 @@
       <c r="A48" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="118">
+      <c r="B48" s="95">
         <v>-41.7</v>
       </c>
-      <c r="C48" s="118">
+      <c r="C48" s="95">
         <v>-79</v>
       </c>
-      <c r="D48" s="118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="118">
+      <c r="D48" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="95">
         <v>-120.7</v>
       </c>
     </row>
@@ -9723,22 +9742,22 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="102" t="s">
+      <c r="A54" s="120" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="100"/>
-      <c r="C54" s="100"/>
-      <c r="D54" s="100"/>
-      <c r="E54" s="101"/>
+      <c r="B54" s="118"/>
+      <c r="C54" s="118"/>
+      <c r="D54" s="118"/>
+      <c r="E54" s="119"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="102" t="s">
+      <c r="A55" s="120" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="100"/>
-      <c r="C55" s="100"/>
-      <c r="D55" s="100"/>
-      <c r="E55" s="101"/>
+      <c r="B55" s="118"/>
+      <c r="C55" s="118"/>
+      <c r="D55" s="118"/>
+      <c r="E55" s="119"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
@@ -9785,10 +9804,10 @@
       <c r="A59" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="121"/>
-      <c r="C59" s="121"/>
-      <c r="D59" s="121"/>
-      <c r="E59" s="121"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="98"/>
+      <c r="D59" s="98"/>
+      <c r="E59" s="98"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
@@ -9902,7 +9921,7 @@
       <c r="C66" s="9">
         <v>956.6</v>
       </c>
-      <c r="D66" s="120" t="s">
+      <c r="D66" s="97" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="9">
@@ -9913,10 +9932,10 @@
       <c r="A67" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B67" s="119"/>
-      <c r="C67" s="119"/>
-      <c r="D67" s="119"/>
-      <c r="E67" s="119"/>
+      <c r="B67" s="96"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="96"/>
+      <c r="E67" s="96"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="27" t="s">
@@ -10041,16 +10060,16 @@
       <c r="A75" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B75" s="118">
+      <c r="B75" s="95">
         <v>59</v>
       </c>
-      <c r="C75" s="118">
+      <c r="C75" s="95">
         <v>456.3</v>
       </c>
-      <c r="D75" s="118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="118">
+      <c r="D75" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="95">
         <v>515.29999999999995</v>
       </c>
     </row>
@@ -10107,13 +10126,13 @@
     </row>
     <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="102" t="s">
+      <c r="A80" s="120" t="s">
         <v>204</v>
       </c>
-      <c r="B80" s="100"/>
-      <c r="C80" s="100"/>
-      <c r="D80" s="100"/>
-      <c r="E80" s="101"/>
+      <c r="B80" s="118"/>
+      <c r="C80" s="118"/>
+      <c r="D80" s="118"/>
+      <c r="E80" s="119"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="27"/>
@@ -10279,16 +10298,16 @@
       <c r="A91" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B91" s="118">
+      <c r="B91" s="95">
         <v>195.5</v>
       </c>
-      <c r="C91" s="118">
+      <c r="C91" s="95">
         <v>359.8</v>
       </c>
-      <c r="D91" s="118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E91" s="118">
+      <c r="D91" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" s="95">
         <v>555.29999999999995</v>
       </c>
     </row>
@@ -10296,10 +10315,10 @@
       <c r="A92" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B92" s="119"/>
-      <c r="C92" s="119"/>
-      <c r="D92" s="119"/>
-      <c r="E92" s="119"/>
+      <c r="B92" s="96"/>
+      <c r="C92" s="96"/>
+      <c r="D92" s="96"/>
+      <c r="E92" s="96"/>
     </row>
     <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="27" t="s">
@@ -10424,16 +10443,16 @@
       <c r="A100" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B100" s="118">
+      <c r="B100" s="95">
         <v>47.5</v>
       </c>
-      <c r="C100" s="118">
+      <c r="C100" s="95">
         <v>45.9</v>
       </c>
-      <c r="D100" s="118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="118">
+      <c r="D100" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="95">
         <v>93.4</v>
       </c>
     </row>
@@ -10522,32 +10541,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="120" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="106" t="s">
+      <c r="B2" s="122"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="106" t="s">
+      <c r="E2" s="125"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="H2" s="108"/>
+      <c r="H2" s="126"/>
     </row>
     <row r="3" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
@@ -10648,32 +10667,32 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="120" t="s">
         <v>208</v>
       </c>
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="118"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
     </row>
     <row r="12" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="104"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106" t="s">
+      <c r="B12" s="122"/>
+      <c r="C12" s="123"/>
+      <c r="D12" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="107"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="106" t="s">
+      <c r="E12" s="125"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="H12" s="108"/>
+      <c r="H12" s="126"/>
     </row>
     <row r="13" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="44" t="s">
@@ -10776,32 +10795,32 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="102" t="s">
+      <c r="A21" s="120" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="100"/>
-      <c r="C21" s="100"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
+      <c r="B21" s="118"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="118"/>
     </row>
     <row r="22" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="104"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="106" t="s">
+      <c r="B22" s="122"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="107"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="106" t="s">
+      <c r="E22" s="125"/>
+      <c r="F22" s="126"/>
+      <c r="G22" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="108"/>
+      <c r="H22" s="126"/>
     </row>
     <row r="23" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
@@ -10902,32 +10921,32 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="102" t="s">
+      <c r="A31" s="120" t="s">
         <v>158</v>
       </c>
-      <c r="B31" s="100"/>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="100"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="118"/>
     </row>
     <row r="32" spans="1:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="103" t="s">
+      <c r="A32" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="104"/>
-      <c r="C32" s="105"/>
-      <c r="D32" s="106" t="s">
+      <c r="B32" s="122"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="107"/>
-      <c r="F32" s="108"/>
-      <c r="G32" s="106" t="s">
+      <c r="E32" s="125"/>
+      <c r="F32" s="126"/>
+      <c r="G32" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="H32" s="108"/>
+      <c r="H32" s="126"/>
     </row>
     <row r="33" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44" t="s">
@@ -11028,32 +11047,32 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="102" t="s">
+      <c r="A41" s="120" t="s">
         <v>159</v>
       </c>
-      <c r="B41" s="100"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="100"/>
-      <c r="E41" s="100"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="100"/>
-      <c r="H41" s="100"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="118"/>
+      <c r="F41" s="118"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="118"/>
     </row>
     <row r="42" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="103" t="s">
+      <c r="A42" s="121" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="104"/>
-      <c r="C42" s="105"/>
-      <c r="D42" s="106" t="s">
+      <c r="B42" s="122"/>
+      <c r="C42" s="123"/>
+      <c r="D42" s="124" t="s">
         <v>116</v>
       </c>
-      <c r="E42" s="107"/>
-      <c r="F42" s="108"/>
-      <c r="G42" s="106" t="s">
+      <c r="E42" s="125"/>
+      <c r="F42" s="126"/>
+      <c r="G42" s="124" t="s">
         <v>117</v>
       </c>
-      <c r="H42" s="108"/>
+      <c r="H42" s="126"/>
     </row>
     <row r="43" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
@@ -11160,7 +11179,6 @@
     <row r="72" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="D42:F42"/>
     <mergeCell ref="G42:H42"/>
@@ -11180,6 +11198,7 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11237,7 +11256,7 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="122" t="s">
+      <c r="E3" s="99" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11254,7 +11273,7 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" s="122" t="s">
+      <c r="E4" s="99" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11271,7 +11290,7 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" s="122" t="s">
+      <c r="E5" s="99" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11279,12 +11298,12 @@
       <c r="A6" s="51"/>
     </row>
     <row r="7" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="120" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="100"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="101"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="119"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
@@ -11377,7 +11396,7 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="E15" s="122" t="s">
+      <c r="E15" s="99" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11419,12 +11438,12 @@
       <c r="A18" s="51"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="102" t="s">
+      <c r="A19" s="120" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="101"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="119"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44" t="s">
@@ -11495,7 +11514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -11513,11 +11532,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="120" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
     </row>
     <row r="3" spans="1:3" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
@@ -11614,7 +11633,7 @@
       <c r="B11" s="9">
         <v>753.6</v>
       </c>
-      <c r="C11" s="120" t="s">
+      <c r="C11" s="97" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11662,11 +11681,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="102" t="s">
+      <c r="A19" s="120" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
     </row>
     <row r="20" spans="1:3" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
@@ -11763,7 +11782,7 @@
       <c r="B28" s="9">
         <v>105.7</v>
       </c>
-      <c r="C28" s="120" t="s">
+      <c r="C28" s="97" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed to handle single line input tabs.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/MEADS/2011_SAR DataDraw_MEADS.xlsx
+++ b/FOIA SAR data/MEADS/2011_SAR DataDraw_MEADS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CostSummary" sheetId="1" r:id="rId1"/>
@@ -1420,11 +1420,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1432,10 +1432,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1450,22 +1471,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1494,12 +1500,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1843,75 +1843,75 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="104"/>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="111" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="107"/>
+      <c r="C3" s="112"/>
       <c r="D3" s="30"/>
       <c r="E3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F3" s="106" t="s">
+      <c r="F3" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="107"/>
-      <c r="H3" s="108"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="115"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="105"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="113"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="114"/>
       <c r="D4" s="31"/>
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="109"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="111"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="118"/>
     </row>
     <row r="5" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="102" t="s">
+      <c r="D5" s="115"/>
+      <c r="E5" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="112"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="114"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="119"/>
     </row>
     <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="115"/>
-      <c r="B6" s="117"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="102" t="s">
+      <c r="A6" s="109"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="102" t="s">
+      <c r="G6" s="106" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="102" t="s">
+      <c r="H6" s="106" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="116"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="108"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -2216,75 +2216,75 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="104"/>
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="111" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="107"/>
-      <c r="D21" s="108"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="115"/>
       <c r="E21" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="F21" s="106" t="s">
+      <c r="F21" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="107"/>
-      <c r="H21" s="108"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="115"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="105"/>
-      <c r="B22" s="112"/>
-      <c r="C22" s="113"/>
-      <c r="D22" s="114"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="119"/>
       <c r="E22" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="109"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="111"/>
+      <c r="F22" s="116"/>
+      <c r="G22" s="117"/>
+      <c r="H22" s="118"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="102" t="s">
+      <c r="A23" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="102" t="s">
+      <c r="B23" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="106" t="s">
+      <c r="C23" s="111" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="108"/>
-      <c r="E23" s="102" t="s">
+      <c r="D23" s="115"/>
+      <c r="E23" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="112"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="114"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="119"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="115"/>
-      <c r="B24" s="117"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="115"/>
-      <c r="F24" s="102" t="s">
+      <c r="A24" s="109"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="102" t="s">
+      <c r="G24" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="H24" s="102" t="s">
+      <c r="H24" s="106" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="116"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="112"/>
-      <c r="D25" s="114"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="116"/>
-      <c r="H25" s="116"/>
+      <c r="A25" s="110"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="110"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
@@ -2587,10 +2587,10 @@
       <c r="B38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="102" t="s">
+      <c r="C38" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="102" t="s">
+      <c r="D38" s="106" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2601,8 +2601,8 @@
       <c r="B39" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="103"/>
-      <c r="D39" s="103"/>
+      <c r="C39" s="108"/>
+      <c r="D39" s="108"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -2659,75 +2659,75 @@
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="104"/>
-      <c r="B46" s="106" t="s">
+      <c r="B46" s="111" t="s">
         <v>161</v>
       </c>
-      <c r="C46" s="107"/>
-      <c r="D46" s="108"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="115"/>
       <c r="E46" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="F46" s="106" t="s">
+      <c r="F46" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="107"/>
-      <c r="H46" s="108"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="115"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="105"/>
-      <c r="B47" s="112"/>
-      <c r="C47" s="113"/>
-      <c r="D47" s="114"/>
+      <c r="B47" s="113"/>
+      <c r="C47" s="114"/>
+      <c r="D47" s="119"/>
       <c r="E47" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="F47" s="109"/>
-      <c r="G47" s="110"/>
-      <c r="H47" s="111"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="117"/>
+      <c r="H47" s="118"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="102" t="s">
+      <c r="A48" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="102" t="s">
+      <c r="B48" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="C48" s="106" t="s">
+      <c r="C48" s="111" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="108"/>
-      <c r="E48" s="102" t="s">
+      <c r="D48" s="115"/>
+      <c r="E48" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="F48" s="112"/>
-      <c r="G48" s="113"/>
-      <c r="H48" s="114"/>
+      <c r="F48" s="113"/>
+      <c r="G48" s="114"/>
+      <c r="H48" s="119"/>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="115"/>
-      <c r="B49" s="117"/>
-      <c r="C49" s="109"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="115"/>
-      <c r="F49" s="102" t="s">
+      <c r="A49" s="109"/>
+      <c r="B49" s="107"/>
+      <c r="C49" s="116"/>
+      <c r="D49" s="118"/>
+      <c r="E49" s="109"/>
+      <c r="F49" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="G49" s="102" t="s">
+      <c r="G49" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="H49" s="102" t="s">
+      <c r="H49" s="106" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="116"/>
-      <c r="B50" s="103"/>
-      <c r="C50" s="112"/>
-      <c r="D50" s="114"/>
-      <c r="E50" s="116"/>
-      <c r="F50" s="116"/>
-      <c r="G50" s="116"/>
-      <c r="H50" s="116"/>
+      <c r="A50" s="110"/>
+      <c r="B50" s="108"/>
+      <c r="C50" s="113"/>
+      <c r="D50" s="119"/>
+      <c r="E50" s="110"/>
+      <c r="F50" s="110"/>
+      <c r="G50" s="110"/>
+      <c r="H50" s="110"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
@@ -3030,10 +3030,10 @@
       <c r="B63" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C63" s="102" t="s">
+      <c r="C63" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="D63" s="102" t="s">
+      <c r="D63" s="106" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3044,8 +3044,8 @@
       <c r="B64" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="103"/>
-      <c r="D64" s="103"/>
+      <c r="C64" s="108"/>
+      <c r="D64" s="108"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
@@ -3091,28 +3091,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="F3:H5"/>
-    <mergeCell ref="C5:D7"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B21:D22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
     <mergeCell ref="C63:C64"/>
     <mergeCell ref="D63:D64"/>
     <mergeCell ref="A46:A47"/>
@@ -3125,6 +3103,28 @@
     <mergeCell ref="G49:G50"/>
     <mergeCell ref="H49:H50"/>
     <mergeCell ref="B46:D47"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="F3:H5"/>
+    <mergeCell ref="C5:D7"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B21:D22"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3135,7 +3135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K944"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3152,45 +3152,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="102" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
       <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
       <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="103" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
       <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3476,32 +3476,32 @@
       <c r="J13" s="63"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="120" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="118"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="119"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="121"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="120" t="s">
         <v>169</v>
       </c>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="119"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="120"/>
+      <c r="E15" s="120"/>
+      <c r="F15" s="120"/>
+      <c r="G15" s="120"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="121"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
@@ -4012,33 +4012,33 @@
       <c r="K32" s="12"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="118" t="s">
+      <c r="A33" s="120" t="s">
         <v>174</v>
       </c>
-      <c r="B33" s="118"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="118"/>
-      <c r="J33" s="119"/>
+      <c r="B33" s="120"/>
+      <c r="C33" s="120"/>
+      <c r="D33" s="120"/>
+      <c r="E33" s="120"/>
+      <c r="F33" s="120"/>
+      <c r="G33" s="120"/>
+      <c r="H33" s="120"/>
+      <c r="I33" s="120"/>
+      <c r="J33" s="121"/>
       <c r="K33" s="12"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="118" t="s">
+      <c r="A34" s="120" t="s">
         <v>169</v>
       </c>
-      <c r="B34" s="118"/>
-      <c r="C34" s="118"/>
-      <c r="D34" s="118"/>
-      <c r="E34" s="118"/>
-      <c r="F34" s="118"/>
-      <c r="G34" s="118"/>
-      <c r="H34" s="118"/>
-      <c r="I34" s="118"/>
-      <c r="J34" s="119"/>
+      <c r="B34" s="120"/>
+      <c r="C34" s="120"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="120"/>
+      <c r="F34" s="120"/>
+      <c r="G34" s="120"/>
+      <c r="H34" s="120"/>
+      <c r="I34" s="120"/>
+      <c r="J34" s="121"/>
       <c r="K34" s="12"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -4557,17 +4557,17 @@
       <c r="K51" s="12"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="118" t="s">
+      <c r="A52" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="B52" s="118"/>
-      <c r="C52" s="118"/>
-      <c r="D52" s="118"/>
-      <c r="E52" s="118"/>
-      <c r="F52" s="118"/>
-      <c r="G52" s="118"/>
-      <c r="H52" s="118"/>
-      <c r="I52" s="119"/>
+      <c r="B52" s="120"/>
+      <c r="C52" s="120"/>
+      <c r="D52" s="120"/>
+      <c r="E52" s="120"/>
+      <c r="F52" s="120"/>
+      <c r="G52" s="120"/>
+      <c r="H52" s="120"/>
+      <c r="I52" s="121"/>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
     </row>
@@ -4895,17 +4895,17 @@
       <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="118" t="s">
+      <c r="A66" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="B66" s="118"/>
-      <c r="C66" s="118"/>
-      <c r="D66" s="118"/>
-      <c r="E66" s="118"/>
-      <c r="F66" s="118"/>
-      <c r="G66" s="118"/>
-      <c r="H66" s="118"/>
-      <c r="I66" s="119"/>
+      <c r="B66" s="120"/>
+      <c r="C66" s="120"/>
+      <c r="D66" s="120"/>
+      <c r="E66" s="120"/>
+      <c r="F66" s="120"/>
+      <c r="G66" s="120"/>
+      <c r="H66" s="120"/>
+      <c r="I66" s="121"/>
     </row>
     <row r="67" spans="1:9" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="27" t="s">
@@ -5231,72 +5231,72 @@
       <c r="H79" s="12"/>
     </row>
     <row r="80" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="118" t="s">
+      <c r="A80" s="120" t="s">
         <v>178</v>
       </c>
-      <c r="B80" s="118"/>
-      <c r="C80" s="118"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="118"/>
-      <c r="F80" s="118"/>
-      <c r="G80" s="118"/>
-      <c r="H80" s="118"/>
+      <c r="B80" s="120"/>
+      <c r="C80" s="120"/>
+      <c r="D80" s="120"/>
+      <c r="E80" s="120"/>
+      <c r="F80" s="120"/>
+      <c r="G80" s="120"/>
+      <c r="H80" s="120"/>
     </row>
     <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="102" t="s">
+      <c r="A81" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="102" t="s">
+      <c r="B81" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="102" t="s">
+      <c r="C81" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="D81" s="102" t="s">
+      <c r="D81" s="106" t="s">
         <v>45</v>
       </c>
-      <c r="E81" s="102" t="s">
+      <c r="E81" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="F81" s="102" t="s">
+      <c r="F81" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="G81" s="102" t="s">
+      <c r="G81" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="H81" s="102" t="s">
+      <c r="H81" s="106" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="117"/>
-      <c r="B82" s="117"/>
-      <c r="C82" s="117"/>
-      <c r="D82" s="117"/>
-      <c r="E82" s="117"/>
-      <c r="F82" s="117"/>
-      <c r="G82" s="117"/>
-      <c r="H82" s="117"/>
+      <c r="A82" s="107"/>
+      <c r="B82" s="107"/>
+      <c r="C82" s="107"/>
+      <c r="D82" s="107"/>
+      <c r="E82" s="107"/>
+      <c r="F82" s="107"/>
+      <c r="G82" s="107"/>
+      <c r="H82" s="107"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="117"/>
-      <c r="B83" s="117"/>
-      <c r="C83" s="117"/>
-      <c r="D83" s="117"/>
-      <c r="E83" s="117"/>
-      <c r="F83" s="117"/>
-      <c r="G83" s="117"/>
-      <c r="H83" s="117"/>
+      <c r="A83" s="107"/>
+      <c r="B83" s="107"/>
+      <c r="C83" s="107"/>
+      <c r="D83" s="107"/>
+      <c r="E83" s="107"/>
+      <c r="F83" s="107"/>
+      <c r="G83" s="107"/>
+      <c r="H83" s="107"/>
     </row>
     <row r="84" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="103"/>
-      <c r="B84" s="103"/>
-      <c r="C84" s="103"/>
-      <c r="D84" s="103"/>
-      <c r="E84" s="103"/>
-      <c r="F84" s="103"/>
-      <c r="G84" s="103"/>
-      <c r="H84" s="103"/>
+      <c r="A84" s="108"/>
+      <c r="B84" s="108"/>
+      <c r="C84" s="108"/>
+      <c r="D84" s="108"/>
+      <c r="E84" s="108"/>
+      <c r="F84" s="108"/>
+      <c r="G84" s="108"/>
+      <c r="H84" s="108"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
@@ -5586,16 +5586,16 @@
     </row>
     <row r="96" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="97" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="118" t="s">
+      <c r="A97" s="120" t="s">
         <v>179</v>
       </c>
-      <c r="B97" s="118"/>
-      <c r="C97" s="118"/>
-      <c r="D97" s="118"/>
-      <c r="E97" s="118"/>
-      <c r="F97" s="118"/>
-      <c r="G97" s="118"/>
-      <c r="H97" s="118"/>
+      <c r="B97" s="120"/>
+      <c r="C97" s="120"/>
+      <c r="D97" s="120"/>
+      <c r="E97" s="120"/>
+      <c r="F97" s="120"/>
+      <c r="G97" s="120"/>
+      <c r="H97" s="120"/>
     </row>
     <row r="98" spans="1:8" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="27" t="s">
@@ -5911,16 +5911,16 @@
     </row>
     <row r="110" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="118" t="s">
+      <c r="A111" s="120" t="s">
         <v>186</v>
       </c>
-      <c r="B111" s="118"/>
-      <c r="C111" s="118"/>
-      <c r="D111" s="118"/>
-      <c r="E111" s="118"/>
-      <c r="F111" s="118"/>
-      <c r="G111" s="118"/>
-      <c r="H111" s="118"/>
+      <c r="B111" s="120"/>
+      <c r="C111" s="120"/>
+      <c r="D111" s="120"/>
+      <c r="E111" s="120"/>
+      <c r="F111" s="120"/>
+      <c r="G111" s="120"/>
+      <c r="H111" s="120"/>
     </row>
     <row r="112" spans="1:8" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="27" t="s">
@@ -6551,16 +6551,16 @@
       <c r="I136" s="69"/>
     </row>
     <row r="137" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="118" t="s">
+      <c r="A137" s="120" t="s">
         <v>187</v>
       </c>
-      <c r="B137" s="118"/>
-      <c r="C137" s="118"/>
-      <c r="D137" s="118"/>
-      <c r="E137" s="118"/>
-      <c r="F137" s="118"/>
-      <c r="G137" s="118"/>
-      <c r="H137" s="118"/>
+      <c r="B137" s="120"/>
+      <c r="C137" s="120"/>
+      <c r="D137" s="120"/>
+      <c r="E137" s="120"/>
+      <c r="F137" s="120"/>
+      <c r="G137" s="120"/>
+      <c r="H137" s="120"/>
       <c r="I137" s="69"/>
     </row>
     <row r="138" spans="1:9" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -7258,12 +7258,6 @@
     <row r="944" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A80:H80"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A34:J34"/>
     <mergeCell ref="A111:H111"/>
     <mergeCell ref="A137:H137"/>
     <mergeCell ref="A66:I66"/>
@@ -7276,6 +7270,12 @@
     <mergeCell ref="F81:F84"/>
     <mergeCell ref="G81:G84"/>
     <mergeCell ref="A97:H97"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A34:J34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7286,8 +7286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7298,11 +7298,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="119"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="121"/>
     </row>
     <row r="2" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
@@ -7364,11 +7364,11 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="120" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="119"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="121"/>
     </row>
     <row r="10" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27"/>
@@ -7726,14 +7726,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="120" t="s">
+      <c r="C25" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="D25" s="119"/>
-      <c r="E25" s="120" t="s">
+      <c r="D25" s="121"/>
+      <c r="E25" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="119"/>
+      <c r="F25" s="121"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="27" t="s">
@@ -7897,17 +7897,17 @@
       <c r="A35" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="120" t="s">
+      <c r="B35" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="119"/>
-      <c r="J35" s="102" t="s">
+      <c r="C35" s="120"/>
+      <c r="D35" s="120"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="120"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="120"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="106" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7939,7 +7939,7 @@
       <c r="I36" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J36" s="103"/>
+      <c r="J36" s="108"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
@@ -7981,17 +7981,17 @@
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="41"/>
-      <c r="B40" s="120" t="s">
+      <c r="B40" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="118"/>
-      <c r="D40" s="118"/>
-      <c r="E40" s="118"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="119"/>
-      <c r="J40" s="102" t="s">
+      <c r="C40" s="120"/>
+      <c r="D40" s="120"/>
+      <c r="E40" s="120"/>
+      <c r="F40" s="120"/>
+      <c r="G40" s="120"/>
+      <c r="H40" s="120"/>
+      <c r="I40" s="121"/>
+      <c r="J40" s="106" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8023,7 +8023,7 @@
       <c r="I41" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J41" s="103"/>
+      <c r="J41" s="108"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
@@ -8064,13 +8064,13 @@
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="120" t="s">
+      <c r="A45" s="122" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="118"/>
-      <c r="C45" s="118"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="119"/>
+      <c r="B45" s="120"/>
+      <c r="C45" s="120"/>
+      <c r="D45" s="120"/>
+      <c r="E45" s="121"/>
     </row>
     <row r="46" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
@@ -8444,14 +8444,14 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C80" s="120" t="s">
+      <c r="C80" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="D80" s="119"/>
-      <c r="E80" s="120" t="s">
+      <c r="D80" s="121"/>
+      <c r="E80" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="F80" s="119"/>
+      <c r="F80" s="121"/>
     </row>
     <row r="81" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="27" t="s">
@@ -8615,17 +8615,17 @@
       <c r="A90" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B90" s="120" t="s">
+      <c r="B90" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="C90" s="118"/>
-      <c r="D90" s="118"/>
-      <c r="E90" s="118"/>
-      <c r="F90" s="118"/>
-      <c r="G90" s="118"/>
-      <c r="H90" s="118"/>
-      <c r="I90" s="119"/>
-      <c r="J90" s="102" t="s">
+      <c r="C90" s="120"/>
+      <c r="D90" s="120"/>
+      <c r="E90" s="120"/>
+      <c r="F90" s="120"/>
+      <c r="G90" s="120"/>
+      <c r="H90" s="120"/>
+      <c r="I90" s="121"/>
+      <c r="J90" s="106" t="s">
         <v>86</v>
       </c>
     </row>
@@ -8657,7 +8657,7 @@
       <c r="I91" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J91" s="103"/>
+      <c r="J91" s="108"/>
     </row>
     <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="27" t="s">
@@ -8699,17 +8699,17 @@
     <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="41"/>
-      <c r="B95" s="120" t="s">
+      <c r="B95" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="C95" s="118"/>
-      <c r="D95" s="118"/>
-      <c r="E95" s="118"/>
-      <c r="F95" s="118"/>
-      <c r="G95" s="118"/>
-      <c r="H95" s="118"/>
-      <c r="I95" s="119"/>
-      <c r="J95" s="102" t="s">
+      <c r="C95" s="120"/>
+      <c r="D95" s="120"/>
+      <c r="E95" s="120"/>
+      <c r="F95" s="120"/>
+      <c r="G95" s="120"/>
+      <c r="H95" s="120"/>
+      <c r="I95" s="121"/>
+      <c r="J95" s="106" t="s">
         <v>89</v>
       </c>
     </row>
@@ -8741,7 +8741,7 @@
       <c r="I96" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="J96" s="103"/>
+      <c r="J96" s="108"/>
     </row>
     <row r="97" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="27" t="s">
@@ -8782,13 +8782,13 @@
     </row>
     <row r="99" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="120" t="s">
+      <c r="A100" s="122" t="s">
         <v>90</v>
       </c>
-      <c r="B100" s="118"/>
-      <c r="C100" s="118"/>
-      <c r="D100" s="118"/>
-      <c r="E100" s="119"/>
+      <c r="B100" s="120"/>
+      <c r="C100" s="120"/>
+      <c r="D100" s="120"/>
+      <c r="E100" s="121"/>
     </row>
     <row r="101" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="27" t="s">
@@ -8971,22 +8971,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="122" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="119"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="121"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="122" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="119"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="121"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27"/>
@@ -9355,13 +9355,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="120" t="s">
+      <c r="A28" s="122" t="s">
         <v>204</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="119"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="121"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="27"/>
@@ -9742,22 +9742,22 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="120" t="s">
+      <c r="A54" s="122" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="118"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="118"/>
-      <c r="E54" s="119"/>
+      <c r="B54" s="120"/>
+      <c r="C54" s="120"/>
+      <c r="D54" s="120"/>
+      <c r="E54" s="121"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="120" t="s">
+      <c r="A55" s="122" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="118"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="118"/>
-      <c r="E55" s="119"/>
+      <c r="B55" s="120"/>
+      <c r="C55" s="120"/>
+      <c r="D55" s="120"/>
+      <c r="E55" s="121"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
@@ -10126,13 +10126,13 @@
     </row>
     <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="120" t="s">
+      <c r="A80" s="122" t="s">
         <v>204</v>
       </c>
-      <c r="B80" s="118"/>
-      <c r="C80" s="118"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="119"/>
+      <c r="B80" s="120"/>
+      <c r="C80" s="120"/>
+      <c r="D80" s="120"/>
+      <c r="E80" s="121"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="27"/>
@@ -10541,32 +10541,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
     </row>
     <row r="2" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="124" t="s">
+      <c r="B2" s="124"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="125"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="124" t="s">
+      <c r="E2" s="127"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="H2" s="126"/>
+      <c r="H2" s="128"/>
     </row>
     <row r="3" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
@@ -10667,32 +10667,32 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="120" t="s">
+      <c r="A11" s="122" t="s">
         <v>208</v>
       </c>
-      <c r="B11" s="118"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
     </row>
     <row r="12" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="122"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="124" t="s">
+      <c r="B12" s="124"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="125"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="124" t="s">
+      <c r="E12" s="127"/>
+      <c r="F12" s="128"/>
+      <c r="G12" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="H12" s="126"/>
+      <c r="H12" s="128"/>
     </row>
     <row r="13" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="44" t="s">
@@ -10795,32 +10795,32 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="120" t="s">
+      <c r="A21" s="122" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="120"/>
+      <c r="F21" s="120"/>
+      <c r="G21" s="120"/>
+      <c r="H21" s="120"/>
     </row>
     <row r="22" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="122"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="124" t="s">
+      <c r="B22" s="124"/>
+      <c r="C22" s="125"/>
+      <c r="D22" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="125"/>
-      <c r="F22" s="126"/>
-      <c r="G22" s="124" t="s">
+      <c r="E22" s="127"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="126"/>
+      <c r="H22" s="128"/>
     </row>
     <row r="23" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
@@ -10921,32 +10921,32 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="120" t="s">
+      <c r="A31" s="122" t="s">
         <v>158</v>
       </c>
-      <c r="B31" s="118"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
+      <c r="B31" s="120"/>
+      <c r="C31" s="120"/>
+      <c r="D31" s="120"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="120"/>
+      <c r="G31" s="120"/>
+      <c r="H31" s="120"/>
     </row>
     <row r="32" spans="1:8" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="121" t="s">
+      <c r="A32" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="122"/>
-      <c r="C32" s="123"/>
-      <c r="D32" s="124" t="s">
+      <c r="B32" s="124"/>
+      <c r="C32" s="125"/>
+      <c r="D32" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="125"/>
-      <c r="F32" s="126"/>
-      <c r="G32" s="124" t="s">
+      <c r="E32" s="127"/>
+      <c r="F32" s="128"/>
+      <c r="G32" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="H32" s="126"/>
+      <c r="H32" s="128"/>
     </row>
     <row r="33" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44" t="s">
@@ -11047,32 +11047,32 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="120" t="s">
+      <c r="A41" s="122" t="s">
         <v>159</v>
       </c>
-      <c r="B41" s="118"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="118"/>
-      <c r="E41" s="118"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="118"/>
-      <c r="H41" s="118"/>
+      <c r="B41" s="120"/>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="120"/>
     </row>
     <row r="42" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="121" t="s">
+      <c r="A42" s="123" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="122"/>
-      <c r="C42" s="123"/>
-      <c r="D42" s="124" t="s">
+      <c r="B42" s="124"/>
+      <c r="C42" s="125"/>
+      <c r="D42" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="E42" s="125"/>
-      <c r="F42" s="126"/>
-      <c r="G42" s="124" t="s">
+      <c r="E42" s="127"/>
+      <c r="F42" s="128"/>
+      <c r="G42" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="H42" s="126"/>
+      <c r="H42" s="128"/>
     </row>
     <row r="43" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
@@ -11179,6 +11179,10 @@
     <row r="72" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="D42:F42"/>
     <mergeCell ref="G42:H42"/>
@@ -11195,10 +11199,6 @@
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11298,12 +11298,12 @@
       <c r="A6" s="51"/>
     </row>
     <row r="7" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="122" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="119"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="121"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
@@ -11438,12 +11438,12 @@
       <c r="A18" s="51"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="120" t="s">
+      <c r="A19" s="122" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
-      <c r="D19" s="119"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
+      <c r="D19" s="121"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44" t="s">
@@ -11532,11 +11532,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="122" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:3" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="46" t="s">
@@ -11681,11 +11681,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="120" t="s">
+      <c r="A19" s="122" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="120"/>
     </row>
     <row r="20" spans="1:3" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">

</xml_diff>